<commit_message>
Fix xml file issues
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_3_2023.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_3_2023.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -449,14 +449,14 @@
       <c r="G2">
         <v>10</v>
       </c>
-      <c r="H2" t="str">
-        <v>--</v>
+      <c r="H2">
+        <v>0</v>
       </c>
       <c r="I2">
         <v>12000</v>
       </c>
-      <c r="J2" t="str">
-        <v>--</v>
+      <c r="J2">
+        <v>600</v>
       </c>
       <c r="K2">
         <v>1200</v>
@@ -467,8 +467,8 @@
       <c r="M2">
         <v>0</v>
       </c>
-      <c r="N2">
-        <v>12000</v>
+      <c r="N2" t="str">
+        <v>--</v>
       </c>
       <c r="O2">
         <v>22800</v>
@@ -476,34 +476,34 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>222/RABAT /AV1</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B3" t="str">
-        <v>Direction régionale</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C3" t="str">
-        <v>K2574857</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D3" t="str">
-        <v>NADIA JJEE</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E3" t="str">
-        <v>non</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="F3" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G3">
-        <v>15</v>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G3" t="str">
+        <v xml:space="preserve"> </v>
       </c>
       <c r="H3">
-        <v>13333.33</v>
+        <v>0</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>2000</v>
+        <v>600</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -514,298 +514,16 @@
       <c r="M3">
         <v>0</v>
       </c>
-      <c r="N3" t="str">
-        <v>--</v>
+      <c r="N3">
+        <v>0</v>
       </c>
       <c r="O3">
-        <v>11333.33</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>222/RABAT /AV1</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Direction régionale</v>
-      </c>
-      <c r="C4" t="str">
-        <v>F4767464</v>
-      </c>
-      <c r="D4" t="str">
-        <v xml:space="preserve">MED FARID </v>
-      </c>
-      <c r="E4" t="str">
-        <v>non</v>
-      </c>
-      <c r="F4" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>1666.67</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4" t="str">
-        <v>--</v>
-      </c>
-      <c r="O4">
-        <v>1666.67</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>222/RABAT /AV1</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Direction régionale</v>
-      </c>
-      <c r="C5" t="str">
-        <v>M564634</v>
-      </c>
-      <c r="D5" t="str">
-        <v>LATIFA FIFA</v>
-      </c>
-      <c r="E5" t="str">
-        <v>non</v>
-      </c>
-      <c r="F5" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G5">
-        <v>10</v>
-      </c>
-      <c r="H5">
-        <v>5000</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>500</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5" t="str">
-        <v>--</v>
-      </c>
-      <c r="O5">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>966/RABAT SUP1/AV1</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Supervision</v>
-      </c>
-      <c r="C6" t="str">
-        <v>L5453746</v>
-      </c>
-      <c r="D6" t="str">
-        <v>MERYEM RARA</v>
-      </c>
-      <c r="E6" t="str">
-        <v>non</v>
-      </c>
-      <c r="F6" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G6">
-        <v>10</v>
-      </c>
-      <c r="H6">
-        <v>3000</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>300</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6" t="str">
-        <v>--</v>
-      </c>
-      <c r="O6">
-        <v>2700</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>966/RABAT SUP1/AV1</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Supervision</v>
-      </c>
-      <c r="C7" t="str">
-        <v>KL254545</v>
-      </c>
-      <c r="D7" t="str">
-        <v>LAILA JJJJ</v>
-      </c>
-      <c r="E7" t="str">
-        <v>non</v>
-      </c>
-      <c r="F7" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G7">
-        <v>10</v>
-      </c>
-      <c r="H7">
-        <v>4500</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>450</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7" t="str">
-        <v>--</v>
-      </c>
-      <c r="O7">
-        <v>4050</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>966/RABAT SUP1/AV1</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Supervision</v>
-      </c>
-      <c r="C8" t="str">
-        <v>354643</v>
-      </c>
-      <c r="D8" t="str">
-        <v>STE LOC 10</v>
-      </c>
-      <c r="E8" t="str">
-        <v>oui</v>
-      </c>
-      <c r="F8" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>7500</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8" t="str">
-        <v>--</v>
-      </c>
-      <c r="O8">
-        <v>7500</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="B9" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C9" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D9" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E9" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F9" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G9" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H9">
-        <v>35000</v>
-      </c>
-      <c r="I9">
-        <v>12000</v>
-      </c>
-      <c r="J9">
-        <v>3250</v>
-      </c>
-      <c r="K9">
-        <v>1200</v>
-      </c>
-      <c r="L9">
-        <v>12000</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>54550</v>
+        <v>22800</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>